<commit_message>
changed deactivate to activate in Configurations.xlsx
</commit_message>
<xml_diff>
--- a/Configurations.xlsx
+++ b/Configurations.xlsx
@@ -50,7 +50,7 @@
     <t>row</t>
   </si>
   <si>
-    <t>deactivate</t>
+    <t>activate</t>
   </si>
 </sst>
 </file>
@@ -370,8 +370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed activate to deactivate in Configurations.xlsx
</commit_message>
<xml_diff>
--- a/Configurations.xlsx
+++ b/Configurations.xlsx
@@ -50,7 +50,7 @@
     <t>row</t>
   </si>
   <si>
-    <t>activate</t>
+    <t>deactivate</t>
   </si>
 </sst>
 </file>
@@ -371,7 +371,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>